<commit_message>
3/8 - Update Project Checklist
3/8 - Update Project Checklist
</commit_message>
<xml_diff>
--- a/Documentation/Project_Checklist.xlsx
+++ b/Documentation/Project_Checklist.xlsx
@@ -5,18 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c049dc3e477e8ff/Documents/MTech/2021-2022 Semester 2/IRS_Practice_Module/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c049dc3e477e8ff/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{809AA8AC-CF5C-49BA-95ED-2551075BA519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D095455C-974D-489E-851D-267503D3DA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{688D9BF9-4096-448A-9E77-9949A016F6B0}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="5" xr2:uid="{688D9BF9-4096-448A-9E77-9949A016F6B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
     <sheet name="Evaluation" sheetId="4" r:id="rId2"/>
     <sheet name="Deliverable Submisson Checklist" sheetId="1" r:id="rId3"/>
     <sheet name="References" sheetId="3" r:id="rId4"/>
+    <sheet name="Report Outline" sheetId="5" r:id="rId5"/>
+    <sheet name="Schedule" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="106">
   <si>
     <t>Business Pain &amp; Value; Use Case Demo; Pricing;</t>
   </si>
@@ -1149,14 +1151,175 @@
     <t>Evaluation Criteria</t>
   </si>
   <si>
-    <t>MVP Project - Requirements (Due 1 May 2022</t>
+    <t>ITEM</t>
+  </si>
+  <si>
+    <t>Executive Summary</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>Knowledge Modeling</t>
+  </si>
+  <si>
+    <t>System Design &amp; Development</t>
+  </si>
+  <si>
+    <t>Data Overview</t>
+  </si>
+  <si>
+    <t>Data Structures</t>
+  </si>
+  <si>
+    <t>Data Flow Diagram</t>
+  </si>
+  <si>
+    <t>Logical Architecture</t>
+  </si>
+  <si>
+    <t>User Interface</t>
+  </si>
+  <si>
+    <t>Technologies and Tools</t>
+  </si>
+  <si>
+    <t>Appendix</t>
+  </si>
+  <si>
+    <t>Data Preprocessing</t>
+  </si>
+  <si>
+    <t>Model Training</t>
+  </si>
+  <si>
+    <t>Molde Testing</t>
+  </si>
+  <si>
+    <t>Problem Statement</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>Evaluation of Success</t>
+  </si>
+  <si>
+    <t>Appendix of report: Project Proposal</t>
+  </si>
+  <si>
+    <t>Appendix of report: Mapped System Functionalities against knowledge, techniques and skills of modular courses: MR, RS, CGS</t>
+  </si>
+  <si>
+    <t>Appendix of report: Installation and User Guide</t>
+  </si>
+  <si>
+    <t>Appendix of report: 1 or 2 pages individual project report per project member, including:</t>
+  </si>
+  <si>
+    <t>WEEK</t>
+  </si>
+  <si>
+    <t>SUBMISSION</t>
+  </si>
+  <si>
+    <t>DATE START</t>
+  </si>
+  <si>
+    <t>DELIVERABLE</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>1. Completion</t>
+  </si>
+  <si>
+    <t>MVP Project - Requirements (Due 1 May 2022)</t>
+  </si>
+  <si>
+    <t>Videos</t>
+  </si>
+  <si>
+    <t>2 - 5 Minutes</t>
+  </si>
+  <si>
+    <t>Must be engaging</t>
+  </si>
+  <si>
+    <t>Should have background music</t>
+  </si>
+  <si>
+    <t>Business Case</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Market Research (Competitors, Market Cap, Data)</t>
+  </si>
+  <si>
+    <t>High-Level Demo</t>
+  </si>
+  <si>
+    <t>Opportunities</t>
+  </si>
+  <si>
+    <t>https://fewstones.com/</t>
+  </si>
+  <si>
+    <t>https://www.animaker.com/</t>
+  </si>
+  <si>
+    <t>IRS-PM-2021-01-16-IS03PT-GRP-SureBoT (Fake News Detector - Essentially Google Search)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=fJNA814xZsY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRS-PM-2021-07-05-IS03FT-Group-10-ASD-QA-Bot </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=3e6autoyVKE</t>
+  </si>
+  <si>
+    <t>IRS-PM-2021-07-05-IS03FT-Group-17-CoVid-Diagnosis-and-Symptoms-Helper (Telemedicine)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=CCPhgDjqObs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (Course Recommender)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=HqXFM_iB2zc</t>
+  </si>
+  <si>
+    <t>Video Editor</t>
+  </si>
+  <si>
+    <t>Good to Great Project References</t>
+  </si>
+  <si>
+    <t>Observations of Submissions</t>
+  </si>
+  <si>
+    <t>- Intermission</t>
+  </si>
+  <si>
+    <t>1. Project Proposal (Problem, Solution, Outcome)
+2. Raw Dataset
+3. Technology Stack &amp; High-Level</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1320,6 +1483,22 @@
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1363,7 +1542,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1404,23 +1583,11 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
@@ -1443,6 +1610,47 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1761,7 +1969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7348E014-0B64-4C74-A93D-BD85E4AB6B83}">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
@@ -1771,7 +1979,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="13" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="31.2">
@@ -1825,8 +2033,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="108.05078125" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.83984375" style="27"/>
+    <col min="1" max="1" width="108.05078125" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.83984375" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1835,42 +2043,42 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="24" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="25" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="25" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="25" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="25" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="25" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="25" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="24" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1883,8 +2091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91491E79-F43A-4164-90C6-6F55D4667F2E}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -1896,7 +2104,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -1907,127 +2115,127 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="20">
+      <c r="A2" s="27">
         <v>1</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="22" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="18" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="20"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="23" t="s">
+      <c r="A3" s="27"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="19" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="20">
+      <c r="A4" s="27">
         <v>2</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="22" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="18" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="20"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="23" t="s">
+      <c r="A5" s="27"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="19" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="24">
+      <c r="A6" s="20">
         <v>3</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="22" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="24">
+      <c r="A7" s="20">
         <v>4</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="18" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="24">
+      <c r="A8" s="20">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="23" t="s">
+      <c r="B8" s="21"/>
+      <c r="C8" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="24">
+      <c r="A9" s="20">
         <v>4.2</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="23" t="s">
+      <c r="B9" s="21"/>
+      <c r="C9" s="19" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="24">
+      <c r="A10" s="20">
         <v>4.3</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="23" t="s">
+      <c r="B10" s="21"/>
+      <c r="C10" s="19" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="24">
+      <c r="A11" s="20">
         <v>5</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="22" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="24">
+      <c r="A12" s="20">
         <v>6</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="22" t="s">
+      <c r="B12" s="21"/>
+      <c r="C12" s="18" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="24">
+      <c r="A13" s="20">
         <v>7</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="22" t="s">
+      <c r="B13" s="21"/>
+      <c r="C13" s="18" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="20">
+      <c r="A14" s="27">
         <v>8</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="22" t="s">
+      <c r="B14" s="28"/>
+      <c r="C14" s="18" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="62.4">
-      <c r="A15" s="20"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="26" t="s">
+      <c r="A15" s="27"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="22" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -2042,7 +2250,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="7"/>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="17" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2065,11 +2273,11 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="6">
@@ -2097,10 +2305,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24861C4E-DA6F-4AF5-8B49-BA8D499F728F}">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2169,8 +2377,130 @@
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="32" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="29"/>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="29"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="29"/>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="29" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="29"/>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="31" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="31" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="29" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2188,5 +2518,291 @@
     <hyperlink ref="A14" r:id="rId11" xr:uid="{35D6A327-211E-4162-A535-A313E5AF906C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId12"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B434A50-BE37-4060-BF66-21EC05A78A3F}">
+  <dimension ref="A1:A23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="101.26171875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939F1B73-09FF-4C80-B8E7-D8BACA5D1835}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="8.83984375" style="34"/>
+    <col min="2" max="3" width="12.578125" style="34" customWidth="1"/>
+    <col min="4" max="4" width="70.578125" style="34" customWidth="1"/>
+    <col min="5" max="16384" width="8.83984375" style="34"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="43.2">
+      <c r="A2" s="35">
+        <v>1</v>
+      </c>
+      <c r="B2" s="36">
+        <v>44626</v>
+      </c>
+      <c r="C2" s="36">
+        <v>44632</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="35">
+        <v>2</v>
+      </c>
+      <c r="B3" s="36">
+        <v>44633</v>
+      </c>
+      <c r="C3" s="36">
+        <v>44639</v>
+      </c>
+      <c r="D3" s="35"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="35">
+        <v>3</v>
+      </c>
+      <c r="B4" s="36">
+        <v>44640</v>
+      </c>
+      <c r="C4" s="36">
+        <v>44646</v>
+      </c>
+      <c r="D4" s="35"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="35">
+        <v>4</v>
+      </c>
+      <c r="B5" s="36">
+        <v>44647</v>
+      </c>
+      <c r="C5" s="36">
+        <v>44653</v>
+      </c>
+      <c r="D5" s="35"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="35">
+        <v>5</v>
+      </c>
+      <c r="B6" s="36">
+        <v>44654</v>
+      </c>
+      <c r="C6" s="36">
+        <v>44660</v>
+      </c>
+      <c r="D6" s="35"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="35">
+        <v>6</v>
+      </c>
+      <c r="B7" s="36">
+        <v>44661</v>
+      </c>
+      <c r="C7" s="36">
+        <v>44667</v>
+      </c>
+      <c r="D7" s="35"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="35">
+        <v>7</v>
+      </c>
+      <c r="B8" s="36">
+        <v>44668</v>
+      </c>
+      <c r="C8" s="36">
+        <v>44674</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="35">
+        <v>8</v>
+      </c>
+      <c r="B9" s="36">
+        <v>44675</v>
+      </c>
+      <c r="C9" s="36">
+        <v>44681</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="36">
+        <v>44682</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>